<commit_message>
did some excel stuff with 2014
</commit_message>
<xml_diff>
--- a/graphs.xlsx
+++ b/graphs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Angels</t>
   </si>
@@ -49,14 +49,31 @@
   </si>
   <si>
     <t>Athletics</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>2014 Wins</t>
+  </si>
+  <si>
+    <t>Sim Championships</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -84,8 +101,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -93,6 +111,521 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sim Championships</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>98.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>94.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>89.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>88.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>88.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>88.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>184762.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>165289.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>157678.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>139568.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97464.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>93634.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42662.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40788.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40077.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38078.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="1"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2123061592"/>
+        <c:axId val="2123058424"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2123061592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Regular Season Wins</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2123058424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2123058424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Championships</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> out of 1 Million</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2123061592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sim Championships (non WC teams)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sim Championships</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.075583552055993"/>
+                  <c:y val="-0.0209716535433071"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>98.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>94.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>184762.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>165289.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>157678.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>139568.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97464.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>93634.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2137028184"/>
+        <c:axId val="-2137030024"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2137028184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Regular Season Wins</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2137030024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2137030024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Championships</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> out of 1 Million</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2137028184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -417,96 +950,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B2">
         <v>98</v>
       </c>
+      <c r="C2">
+        <v>184762</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
         <v>1</v>
-      </c>
-      <c r="B2">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>2</v>
       </c>
       <c r="B3">
         <v>96</v>
       </c>
+      <c r="C3">
+        <v>165289</v>
+      </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>96</v>
+      </c>
+      <c r="C4">
+        <v>157678</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>94</v>
       </c>
+      <c r="C5">
+        <v>139568</v>
+      </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>4</v>
-      </c>
-      <c r="B5">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>5</v>
       </c>
       <c r="B6">
         <v>90</v>
       </c>
+      <c r="C6">
+        <v>97464</v>
+      </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>90</v>
+      </c>
+      <c r="C7">
+        <v>93634</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>89</v>
       </c>
+      <c r="C8">
+        <v>42662</v>
+      </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
         <v>7</v>
-      </c>
-      <c r="B8">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>8</v>
       </c>
       <c r="B9">
         <v>88</v>
       </c>
+      <c r="C9">
+        <v>40788</v>
+      </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>88</v>
+      </c>
+      <c r="C10">
+        <v>40077</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>88</v>
+      </c>
+      <c r="C11">
+        <v>38078</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>